<commit_message>
Correção no modelo de importação de alunos_dados_cursos
</commit_message>
<xml_diff>
--- a/modelos/aluno_dados_cursos.xlsx
+++ b/modelos/aluno_dados_cursos.xlsx
@@ -43,12 +43,6 @@
     <t>Turno</t>
   </si>
   <si>
-    <t>1 -Matutino
-2 - Vespertino
-3 - Noturno
-4 -  Integral</t>
-  </si>
-  <si>
     <t>2 – Cursando
 3 – Matrícula trancada
 4 – Desvinculado do curso
@@ -89,6 +83,13 @@
   </si>
   <si>
     <t>Código do Curso</t>
+  </si>
+  <si>
+    <t>1 ­ Matutino
+2 ­ Vespertino
+3 ­ Noturno
+4 ­ Integral
+5 ­ EAD</t>
   </si>
 </sst>
 </file>
@@ -589,28 +590,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
@@ -639,26 +640,26 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>4</v>

</xml_diff>